<commit_message>
Atualização automática de SANTO_ANTONIO_DAS_MISSOES.xlsx
</commit_message>
<xml_diff>
--- a/SANTO_ANTONIO_DAS_MISSOES.xlsx
+++ b/SANTO_ANTONIO_DAS_MISSOES.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gera-fichas\Comarcas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{13D03E58-F416-4053-8D65-928D00FABB1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9B13B285-339A-4FBF-9534-6846FAF02170}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1286,7 +1286,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="1" xr:uid="{D868C5DC-9E56-4A99-A795-2DD8A8322314}"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{4D7F3555-4DFC-4367-A8B9-D98EEA4FDED7}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1316,10 +1316,10 @@
         <xdr:cNvPr id="2" name="Chart1" title="Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A216D570-E529-4FEE-926A-4CCF4566E75D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{50BFA1AF-B862-4BD0-A7D1-F0E5A69D5704}"/>
             </a:ext>
             <a:ext uri="GoogleSheetsCustomDataVersion1">
-              <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="" pictureOfChart="1"/>
+              <go:sheetsCustomData xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:go="http://customooxmlschemas.google.com/" pictureOfChart="1"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1357,7 +1357,7 @@
         <xdr:cNvPr id="3" name="Shape 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A91B74DE-6236-4E68-B27F-FBC1C541B87B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B496C203-0F91-40A1-8797-C88829C4ED00}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1420,7 +1420,7 @@
         <xdr:cNvPr id="4" name="Shape 2" title="Desenho">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B6997BFB-7E9C-408F-B379-51437803FD3A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DF6BA69C-F24E-4814-A530-CFD883D5F131}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1439,7 +1439,7 @@
           <xdr:cNvPr id="5" name="Shape 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C1EE255F-557A-3C3C-D42F-CC461C2CC635}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B06F7369-F619-38E5-7F66-F58EED286952}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1488,7 +1488,7 @@
           <xdr:cNvPr id="6" name="Shape 5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1AE027D2-52F7-D486-2B45-C8155114F560}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9C6513C3-D88B-9143-B708-BC8B5A39CA80}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1507,7 +1507,7 @@
             <xdr:cNvPr id="7" name="Shape 6">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7FF416FC-CE1E-8F99-9BBF-00D503A8E1CE}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D2B47CF6-6C97-C0CA-7F7D-E4BB4C0D6606}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1538,7 +1538,7 @@
             <xdr:cNvPr id="8" name="Shape 7">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{75CA597A-4429-5294-F68A-403DADDFCB33}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C1D52A24-E7BA-5CE0-7D5E-A34AE7F444DD}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1569,7 +1569,7 @@
             <xdr:cNvPr id="9" name="Shape 8">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{15C18F7A-48B3-A664-6AA0-9B2C38D0F2D9}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9E5AB7A1-4A04-E736-C011-BBD835E459B8}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1612,7 +1612,7 @@
         <xdr:cNvPr id="10" name="image2.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7C6887BD-1E67-4770-819D-59E1E79B27CD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{825F4E71-D184-45E8-9B5B-85BB6909567B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1650,7 +1650,7 @@
         <xdr:cNvPr id="11" name="image1.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A981DED6-8705-429D-B67E-1EFD5ED42F55}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4FA2F7BB-BA5F-4F5A-A5A1-6835347D81FD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1693,7 +1693,7 @@
         <xdr:cNvPr id="12" name="Imagem 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E9819BA7-81AA-4433-895C-FDE244D5E5C6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C2B22C4F-5276-4782-A40D-78E62DEF5D06}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2006,7 +2006,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC8BD8C7-DAA0-40CD-8F57-E282CAF7F8D3}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD03D959-6574-426B-AAB7-3EA1C38D9C53}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>

</xml_diff>